<commit_message>
IKS012 and edits to inventory
</commit_message>
<xml_diff>
--- a/metadata/Inventory_Iksvaku.xlsx
+++ b/metadata/Inventory_Iksvaku.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="4660" windowWidth="25480" windowHeight="9100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="560" windowWidth="25480" windowHeight="9100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="644" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="336">
   <si>
     <t>(Faces:) Lines</t>
   </si>
@@ -625,9 +625,6 @@
     <t>Sankaranarayanan; Raghunath</t>
   </si>
   <si>
-    <t>Vogel C4 (EI Vol. XX, p. 20, plate C4)</t>
-  </si>
-  <si>
     <t>Vogel B2 (EI Vol. XX, p. 18, plate B2)</t>
   </si>
   <si>
@@ -1063,16 +1060,28 @@
     <t>Vogel, Prakrit Inscriptions from a Buddhist Site at Nagarjunakonda, C3 (EI Vol. XX, pp. 15-17, plate C3); Raghunath 2001: 72 no. 4</t>
   </si>
   <si>
-    <t>Vogel C2 (EI Vol. XX, p. 19f., plate C2); Raghunath 2001: 74 no. 5</t>
-  </si>
-  <si>
     <t>Vogel 1929-30: 17 (C1). — Raghunath 2001: 76-7 (6).</t>
   </si>
   <si>
-    <t>The rubbings shown by Raghunath under his 5 and 6 together belong to our IKS005. No rubbing for our IKS006 in Raghunath.</t>
-  </si>
-  <si>
     <t>Naga 6</t>
+  </si>
+  <si>
+    <t>Naga 15</t>
+  </si>
+  <si>
+    <t>Vogel 1929-30: 20 (C4). — Raghunath 2001: 87-8 (9).</t>
+  </si>
+  <si>
+    <t>Naga 14</t>
+  </si>
+  <si>
+    <t>The rubbings shown by Raghunath under his 5 and 6 together belong to our IKS005.</t>
+  </si>
+  <si>
+    <t>Vogel 1929-30: 19-20 (C2); Raghunath 2001: 74 (5).</t>
+  </si>
+  <si>
+    <t>No rubbing for our IKS006 in Raghunath. See remark under IKS005.</t>
   </si>
 </sst>
 </file>
@@ -1520,8 +1529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E11" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1544,7 +1553,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="64" x14ac:dyDescent="0.2">
@@ -1554,16 +1563,16 @@
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>297</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>287</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>298</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>288</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>9</v>
@@ -1612,10 +1621,10 @@
         <v>4</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>11</v>
@@ -1630,7 +1639,7 @@
         <v>188</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="N4" s="4"/>
     </row>
@@ -1652,25 +1661,25 @@
         <v>15</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>170</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="N5" s="4"/>
     </row>
@@ -1692,16 +1701,16 @@
         <v>4</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>16</v>
@@ -1710,7 +1719,7 @@
         <v>189</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N6" s="4"/>
     </row>
@@ -1726,19 +1735,19 @@
         <v>1</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F7" s="4">
         <v>13</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>17</v>
@@ -1747,48 +1756,50 @@
         <v>171</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="N7" s="4"/>
     </row>
-    <row r="8" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" s="4">
+    <row r="8" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+      <c r="A8" s="5">
         <v>5</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="5">
         <v>5</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="4">
-        <v>14</v>
+      <c r="D8" s="5" t="s">
+        <v>332</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="F8" s="4">
+        <v>305</v>
+      </c>
+      <c r="F8" s="5">
         <v>12</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="L8" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="M8" s="4" t="s">
-        <v>329</v>
-      </c>
-      <c r="N8" s="4"/>
-    </row>
-    <row r="9" spans="1:14" ht="96" x14ac:dyDescent="0.2">
+      <c r="L8" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="M8" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="N8" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="5">
         <v>6</v>
       </c>
@@ -1797,22 +1808,22 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F9" s="5">
         <v>13</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>18</v>
@@ -1821,10 +1832,10 @@
         <v>171</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -1836,22 +1847,22 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F10" s="5">
         <v>5</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>19</v>
@@ -1860,10 +1871,10 @@
         <v>18</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="N10" s="4"/>
     </row>
@@ -1876,31 +1887,31 @@
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F11" s="5">
         <v>7</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>21</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="N11" s="4"/>
     </row>
@@ -1913,32 +1924,32 @@
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F12" s="4">
         <v>9</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>108</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>21</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="N12" s="4"/>
     </row>
@@ -1951,31 +1962,31 @@
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F13" s="5">
         <v>7</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>21</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="N13" s="4"/>
     </row>
@@ -1987,20 +1998,20 @@
         <v>152</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F14" s="5">
         <v>10</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>108</v>
@@ -2009,47 +2020,47 @@
         <v>23</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="N14" s="4"/>
     </row>
     <row r="15" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A15" s="4">
+      <c r="A15" s="5">
         <v>12</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B15" s="5">
         <v>9</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15" s="4">
-        <v>15</v>
+      <c r="D15" s="5" t="s">
+        <v>330</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>306</v>
-      </c>
-      <c r="F15" s="4">
+        <v>305</v>
+      </c>
+      <c r="F15" s="5">
         <v>8</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>10</v>
+        <v>262</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>299</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="L15" s="4" t="s">
-        <v>229</v>
-      </c>
-      <c r="M15" s="4" t="s">
-        <v>190</v>
+      <c r="L15" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="M15" s="5" t="s">
+        <v>331</v>
       </c>
       <c r="N15" s="4"/>
     </row>
@@ -2063,7 +2074,7 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F16" s="4">
         <v>9</v>
@@ -2079,7 +2090,7 @@
         <v>18</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>22</v>
@@ -2096,7 +2107,7 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F17" s="4">
         <v>10</v>
@@ -2112,7 +2123,7 @@
         <v>18</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>22</v>
@@ -2131,28 +2142,28 @@
         <v>11</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F18" s="4">
         <v>7</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N18" s="4"/>
     </row>
@@ -2166,7 +2177,7 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F19" s="4">
         <v>10</v>
@@ -2182,7 +2193,7 @@
         <v>25</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>22</v>
@@ -2199,7 +2210,7 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F20" s="4">
         <v>9</v>
@@ -2215,7 +2226,7 @@
         <v>13</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M20" s="4" t="s">
         <v>22</v>
@@ -2232,7 +2243,7 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F21" s="4">
         <v>10</v>
@@ -2248,7 +2259,7 @@
         <v>23</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>22</v>
@@ -2265,7 +2276,7 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F22" s="4">
         <v>6</v>
@@ -2281,7 +2292,7 @@
         <v>13</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>22</v>
@@ -2308,7 +2319,7 @@
         <v>28</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>10</v>
@@ -2320,10 +2331,10 @@
         <v>29</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="N23" s="4"/>
     </row>
@@ -2355,10 +2366,10 @@
         <v>30</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>31</v>
@@ -2393,7 +2404,7 @@
         <v>171</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>31</v>
@@ -2428,7 +2439,7 @@
         <v>171</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="N26" s="4" t="s">
         <v>31</v>
@@ -2463,7 +2474,7 @@
         <v>172</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>31</v>
@@ -2500,7 +2511,7 @@
         <v>172</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>31</v>
@@ -2537,7 +2548,7 @@
         <v>172</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>31</v>
@@ -2562,12 +2573,12 @@
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N30" s="4"/>
     </row>
@@ -2589,22 +2600,22 @@
         <v>2</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="K31" s="4" t="s">
         <v>181</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N31" s="4"/>
     </row>
@@ -2633,16 +2644,16 @@
         <v>113</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>36</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N32" s="4"/>
     </row>
@@ -2674,10 +2685,10 @@
         <v>24</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N33" s="4"/>
     </row>
@@ -2706,11 +2717,11 @@
         <v>115</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="N34" s="4" t="s">
         <v>175</v>
@@ -2743,7 +2754,7 @@
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>174</v>
@@ -2774,11 +2785,11 @@
         <v>38</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="L36" s="4"/>
       <c r="M36" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>176</v>
@@ -2848,7 +2859,7 @@
         <v>171</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N38" s="4" t="s">
         <v>31</v>
@@ -2880,10 +2891,10 @@
       </c>
       <c r="K39" s="4"/>
       <c r="L39" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N39" s="4" t="s">
         <v>31</v>
@@ -2918,7 +2929,7 @@
         <v>177</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N40" s="4" t="s">
         <v>31</v>
@@ -2953,7 +2964,7 @@
         <v>171</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="N41" s="4" t="s">
         <v>31</v>
@@ -2984,13 +2995,13 @@
         <v>111</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L42" s="4" t="s">
         <v>171</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="N42" s="4"/>
     </row>
@@ -3022,10 +3033,10 @@
         <v>43</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N43" s="4"/>
     </row>
@@ -3056,7 +3067,7 @@
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
       <c r="M44" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="N44" s="4"/>
     </row>
@@ -3089,7 +3100,7 @@
         <v>171</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>31</v>
@@ -3124,7 +3135,7 @@
         <v>171</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="N46" s="4"/>
     </row>
@@ -3140,28 +3151,28 @@
         <v>44</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F47" s="4">
         <v>10</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="K47" s="4" t="s">
         <v>44</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="N47" s="4"/>
     </row>
@@ -3177,7 +3188,7 @@
         <v>43</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F48" s="4">
         <v>14</v>
@@ -3193,10 +3204,10 @@
         <v>32</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="N48" s="4"/>
     </row>
@@ -3212,7 +3223,7 @@
         <v>42</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="F49" s="4">
         <v>8</v>
@@ -3228,10 +3239,10 @@
         <v>45</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="N49" s="4"/>
     </row>
@@ -3253,7 +3264,7 @@
         <v>17</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>10</v>
@@ -3265,10 +3276,10 @@
         <v>183</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>31</v>
@@ -3292,7 +3303,7 @@
         <v>17</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>10</v>
@@ -3307,7 +3318,7 @@
         <v>177</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>31</v>
@@ -3322,16 +3333,16 @@
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F52" s="4">
         <v>12</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>10</v>
@@ -3349,7 +3360,7 @@
         <v>178</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="N52" s="4"/>
     </row>
@@ -3379,10 +3390,10 @@
         <v>50</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="N53" s="4" t="s">
         <v>51</v>
@@ -3406,7 +3417,7 @@
         <v>14</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>10</v>
@@ -3418,10 +3429,10 @@
         <v>54</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="N54" s="4"/>
     </row>
@@ -3441,7 +3452,7 @@
         <v>7</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>10</v>
@@ -3453,10 +3464,10 @@
         <v>55</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="N55" s="4"/>
     </row>
@@ -3476,7 +3487,7 @@
         <v>12</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H56" s="4" t="s">
         <v>61</v>
@@ -3486,10 +3497,10 @@
       </c>
       <c r="K56" s="4"/>
       <c r="L56" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="N56" s="4"/>
     </row>
@@ -3511,7 +3522,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H57" s="4" t="s">
         <v>61</v>
@@ -3523,10 +3534,10 @@
         <v>58</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="N57" s="4"/>
     </row>
@@ -3557,7 +3568,7 @@
       </c>
       <c r="L58" s="4"/>
       <c r="M58" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="N58" s="4"/>
     </row>
@@ -3588,7 +3599,7 @@
         <v>177</v>
       </c>
       <c r="M59" s="4" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="N59" s="4"/>
     </row>
@@ -3621,7 +3632,7 @@
         <v>177</v>
       </c>
       <c r="M60" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N60" s="4"/>
     </row>
@@ -3637,26 +3648,26 @@
         <v>10</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F61" s="4">
         <v>6</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H61" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="K61" s="4"/>
       <c r="L61" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="N61" s="4"/>
     </row>
@@ -3691,7 +3702,7 @@
         <v>179</v>
       </c>
       <c r="M62" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="N62" s="4"/>
     </row>
@@ -3726,7 +3737,7 @@
         <v>177</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N63" s="4"/>
     </row>
@@ -3758,10 +3769,10 @@
         <v>70</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="N64" s="4"/>
     </row>
@@ -3792,7 +3803,7 @@
         <v>177</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="N65" s="4"/>
     </row>
@@ -3825,7 +3836,7 @@
         <v>177</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N66" s="4"/>
     </row>
@@ -3860,7 +3871,7 @@
         <v>177</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N67" s="4"/>
     </row>
@@ -3917,7 +3928,7 @@
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
       <c r="M69" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N69" s="4"/>
     </row>
@@ -3944,7 +3955,7 @@
       <c r="K70" s="4"/>
       <c r="L70" s="4"/>
       <c r="M70" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="N70" s="4"/>
     </row>
@@ -3964,7 +3975,7 @@
         <v>5</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H71" s="4" t="s">
         <v>10</v>
@@ -3976,10 +3987,10 @@
         <v>76</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="N71" s="4"/>
     </row>
@@ -4007,7 +4018,7 @@
         <v>77</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M72" s="4" t="s">
         <v>180</v>
@@ -4043,7 +4054,7 @@
         <v>177</v>
       </c>
       <c r="M73" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N73" s="4"/>
     </row>
@@ -4076,7 +4087,7 @@
         <v>177</v>
       </c>
       <c r="M74" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N74" s="4"/>
     </row>
@@ -4109,7 +4120,7 @@
         <v>177</v>
       </c>
       <c r="M75" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="N75" s="4"/>
     </row>
@@ -4142,7 +4153,7 @@
         <v>177</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N76" s="4"/>
     </row>
@@ -4177,7 +4188,7 @@
         <v>177</v>
       </c>
       <c r="M77" s="4" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="N77" s="4"/>
     </row>
@@ -4207,10 +4218,10 @@
         <v>82</v>
       </c>
       <c r="L78" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M78" s="4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N78" s="4"/>
     </row>
@@ -4243,7 +4254,7 @@
         <v>177</v>
       </c>
       <c r="M79" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="N79" s="4"/>
     </row>
@@ -4265,7 +4276,7 @@
         <v>5</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H80" s="4" t="s">
         <v>61</v>
@@ -4278,10 +4289,10 @@
         <v>177</v>
       </c>
       <c r="M80" s="4" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="N80" s="4" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -4309,7 +4320,7 @@
       </c>
       <c r="L81" s="4"/>
       <c r="M81" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N81" s="4"/>
     </row>
@@ -4325,7 +4336,7 @@
         <v>48</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F82" s="4">
         <v>3</v>
@@ -4339,10 +4350,10 @@
         <v>85</v>
       </c>
       <c r="L82" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="M82" s="4" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N82" s="4" t="s">
         <v>31</v>
@@ -4366,20 +4377,20 @@
         <v>2</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H83" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="K83" s="4" t="s">
         <v>87</v>
       </c>
       <c r="L83" s="4"/>
       <c r="M83" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="N83" s="4"/>
     </row>
@@ -4401,7 +4412,7 @@
         <v>1</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H84" s="4" t="s">
         <v>10</v>
@@ -4414,7 +4425,7 @@
       </c>
       <c r="L84" s="4"/>
       <c r="M84" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="N84" s="4"/>
     </row>
@@ -4443,16 +4454,16 @@
         <v>139</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="K85" s="4" t="s">
         <v>91</v>
       </c>
       <c r="L85" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="M85" s="4" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N85" s="4"/>
     </row>
@@ -4484,10 +4495,10 @@
         <v>92</v>
       </c>
       <c r="L86" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M86" s="4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="N86" s="4"/>
     </row>
@@ -4517,10 +4528,10 @@
         <v>94</v>
       </c>
       <c r="L87" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M87" s="4" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N87" s="4" t="s">
         <v>26</v>
@@ -4549,7 +4560,7 @@
       <c r="K88" s="4"/>
       <c r="L88" s="4"/>
       <c r="M88" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N88" s="4"/>
     </row>
@@ -4576,7 +4587,7 @@
       <c r="K89" s="4"/>
       <c r="L89" s="4"/>
       <c r="M89" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N89" s="4"/>
     </row>
@@ -4603,7 +4614,7 @@
       <c r="K90" s="4"/>
       <c r="L90" s="4"/>
       <c r="M90" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N90" s="4" t="s">
         <v>99</v>
@@ -4632,7 +4643,7 @@
       <c r="K91" s="4"/>
       <c r="L91" s="4"/>
       <c r="M91" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N91" s="4" t="s">
         <v>99</v>
@@ -4661,7 +4672,7 @@
       <c r="K92" s="4"/>
       <c r="L92" s="4"/>
       <c r="M92" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N92" s="4" t="s">
         <v>99</v>
@@ -4688,7 +4699,7 @@
       <c r="K93" s="4"/>
       <c r="L93" s="4"/>
       <c r="M93" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N93" s="4" t="s">
         <v>99</v>
@@ -4715,7 +4726,7 @@
       <c r="K94" s="4"/>
       <c r="L94" s="4"/>
       <c r="M94" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N94" s="4" t="s">
         <v>99</v>
@@ -4744,7 +4755,7 @@
       <c r="K95" s="4"/>
       <c r="L95" s="4"/>
       <c r="M95" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N95" s="4" t="s">
         <v>31</v>
@@ -4798,7 +4809,7 @@
       <c r="K97" s="4"/>
       <c r="L97" s="4"/>
       <c r="M97" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N97" s="4"/>
     </row>
@@ -4823,7 +4834,7 @@
       <c r="K98" s="4"/>
       <c r="L98" s="4"/>
       <c r="M98" s="4" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="N98" s="4" t="s">
         <v>31</v>
@@ -4858,7 +4869,7 @@
       </c>
       <c r="L99" s="4"/>
       <c r="M99" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="N99" s="4"/>
     </row>
@@ -4887,7 +4898,7 @@
         <v>147</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K100" s="4" t="s">
         <v>186</v>
@@ -4896,7 +4907,7 @@
         <v>171</v>
       </c>
       <c r="M100" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="N100" s="4"/>
     </row>
@@ -4925,7 +4936,7 @@
         <v>104</v>
       </c>
       <c r="J101" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K101" s="4" t="s">
         <v>187</v>
@@ -4934,7 +4945,7 @@
         <v>171</v>
       </c>
       <c r="M101" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="N101" s="4"/>
     </row>
@@ -4963,14 +4974,14 @@
         <v>104</v>
       </c>
       <c r="J102" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K102" s="4"/>
       <c r="L102" s="4" t="s">
         <v>171</v>
       </c>
       <c r="M102" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="N102" s="4"/>
     </row>
@@ -4997,14 +5008,14 @@
         <v>104</v>
       </c>
       <c r="J103" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="K103" s="4"/>
       <c r="L103" s="4" t="s">
         <v>171</v>
       </c>
       <c r="M103" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="N103" s="4" t="s">
         <v>31</v>
@@ -5032,7 +5043,7 @@
       </c>
       <c r="K104" s="4"/>
       <c r="L104" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M104" s="4" t="s">
         <v>22</v>
@@ -5049,7 +5060,7 @@
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
       <c r="E105" s="4" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="F105" s="4">
         <v>6</v>
@@ -5061,7 +5072,7 @@
       </c>
       <c r="K105" s="4"/>
       <c r="L105" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M105" s="4" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
edits to texts and inventory
</commit_message>
<xml_diff>
--- a/metadata/Inventory_Iksvaku.xlsx
+++ b/metadata/Inventory_Iksvaku.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="560" windowWidth="25480" windowHeight="9100" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="4660" windowWidth="25480" windowHeight="9100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="351">
   <si>
     <t>(Faces:) Lines</t>
   </si>
@@ -538,9 +538,6 @@
   </si>
   <si>
     <t>59A</t>
-  </si>
-  <si>
-    <t>Sankaranarayanan</t>
   </si>
   <si>
     <t>Vogel</t>
@@ -622,9 +619,6 @@
     <t>Sarkar; Raghunath</t>
   </si>
   <si>
-    <t>Sankaranarayanan; Raghunath</t>
-  </si>
-  <si>
     <t>Vogel B2 (EI Vol. XX, p. 18, plate B2)</t>
   </si>
   <si>
@@ -815,9 +809,6 @@
     <t>ARIE, 1959-60, p. 51</t>
   </si>
   <si>
-    <t>Subrahmanyam Ep. And. I, pp. 146 ff; A. W. Khan-N. Ramesan, A Monograph on an Early Buddhist Stupa at Kesanapalli, p. 4, No. 16, plate XXIII; S. Sankaranarayanam, Kesanapalli Inscription of Chantamula, Year 13 (EI Vol. XXXVIII, pp. 313-318)</t>
-  </si>
-  <si>
     <t>60 (length)</t>
   </si>
   <si>
@@ -931,9 +922,6 @@
     <t>H. K. Narasimhaswami, Nagarjunakonda Image Inscription (EI Vol. XXIX, pp. 137-139)</t>
   </si>
   <si>
-    <t>Sankaranarayanan( EI Vol. XXXVII, part I, pp. 31 ff.)</t>
-  </si>
-  <si>
     <t>Raghunath no.</t>
   </si>
   <si>
@@ -1036,9 +1024,6 @@
     <t>—</t>
   </si>
   <si>
-    <t>nil</t>
-  </si>
-  <si>
     <t>Raghunath 2001: 85-6 (8A).</t>
   </si>
   <si>
@@ -1057,9 +1042,6 @@
     <t>Vogel 1929-30: 20-1 (C5). — Raghunath 2001: 80-1 (6A).</t>
   </si>
   <si>
-    <t>Vogel, Prakrit Inscriptions from a Buddhist Site at Nagarjunakonda, C3 (EI Vol. XX, pp. 15-17, plate C3); Raghunath 2001: 72 no. 4</t>
-  </si>
-  <si>
     <t>Vogel 1929-30: 17 (C1). — Raghunath 2001: 76-7 (6).</t>
   </si>
   <si>
@@ -1082,13 +1064,194 @@
   </si>
   <si>
     <t>No rubbing for our IKS006 in Raghunath. See remark under IKS005.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Corps)"/>
+      </rPr>
+      <t>estampage Leiden N10. —</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vogel; Raghunath</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Corps)"/>
+      </rPr>
+      <t>estampage Leiden N15. —</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Raghunath</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Corps)"/>
+      </rPr>
+      <t xml:space="preserve">estampage Leiden N11. — </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Raghunath</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Corps)"/>
+      </rPr>
+      <t xml:space="preserve">estampage Leiden N11. — </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vogel; Raghunath</t>
+    </r>
+  </si>
+  <si>
+    <t>estampage Leiden N6. — Vogel; Raghunath</t>
+  </si>
+  <si>
+    <t>estampage Leiden N6. — Vogel.</t>
+  </si>
+  <si>
+    <t>estampage Leiden N6 (bottom), N7 (top). — Vogel; Raghunath</t>
+  </si>
+  <si>
+    <t>No plate in Raghunath 2001.</t>
+  </si>
+  <si>
+    <t>Vogel 1929-30: 15-7 (C3). — Raghunath 2001: 72 (4).</t>
+  </si>
+  <si>
+    <t>estampage Leiden N7. — Vogel.</t>
+  </si>
+  <si>
+    <t>estampage Leiden N7. — Vogel; Raghunath.</t>
+  </si>
+  <si>
+    <t>estampage Leiden N8. — Vogel; Raghunath</t>
+  </si>
+  <si>
+    <t>Leiden N8 contains two estampages of the same inscription.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Corps)"/>
+      </rPr>
+      <t xml:space="preserve">estampage Leiden N8. — </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vogel; Raghunath</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Corps)"/>
+      </rPr>
+      <t xml:space="preserve">estampage Leiden N9. — </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Raghunath</t>
+    </r>
+  </si>
+  <si>
+    <t>estampage Leiden N8.</t>
+  </si>
+  <si>
+    <t>Sankaranarayanan; Raghunath.</t>
+  </si>
+  <si>
+    <t>Sankaranarayanan.</t>
+  </si>
+  <si>
+    <t>Sankaranarayanan 1967-8: 31-2. — Raghunath 2001: 69  (2).</t>
+  </si>
+  <si>
+    <t>Kesa 16</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Subrahmanyam Ep. And. I, pp. 146 ff; A. W. Khan-N. Ramesan, A Monograph on an Early Buddhist Stupa at Kesanapalli, p. 4, No. 16, plate XXIII; S. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Corps)"/>
+      </rPr>
+      <t>Sankaranarayanan 1969-70: 317-8. — Raghunath 2001: 70-1 (3).</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1135,19 +1298,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Corps)"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1188,7 +1350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1529,8 +1691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="83" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1553,26 +1715,26 @@
   <sheetData>
     <row r="1" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="E2" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>9</v>
@@ -1621,10 +1783,10 @@
         <v>4</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>11</v>
@@ -1636,10 +1798,10 @@
         <v>13</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="N4" s="4"/>
     </row>
@@ -1653,112 +1815,118 @@
       <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>315</v>
+      </c>
       <c r="E5" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="5">
         <v>15</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>304</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="N5" s="4"/>
+        <v>300</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="6" spans="1:14" ht="112" x14ac:dyDescent="0.2">
-      <c r="A6" s="4">
+      <c r="A6" s="5">
         <v>3</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="5">
         <v>3</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4">
-        <v>16</v>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>349</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="5">
         <v>4</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="L6" s="4" t="s">
-        <v>189</v>
+      <c r="L6" s="5" t="s">
+        <v>346</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>253</v>
+        <v>350</v>
       </c>
       <c r="N6" s="4"/>
     </row>
-    <row r="7" spans="1:14" ht="64" x14ac:dyDescent="0.2">
-      <c r="A7" s="4">
+    <row r="7" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="5">
         <v>4</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="5">
         <v>4</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="4">
+      <c r="D7" s="5">
         <v>1</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F7" s="5">
+        <v>13</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>305</v>
-      </c>
-      <c r="F7" s="4">
-        <v>13</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>299</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>309</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="N7" s="4"/>
+      <c r="L7" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="M7" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="8" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="5">
@@ -1769,34 +1937,34 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="5" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F8" s="5">
         <v>12</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>20</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>228</v>
+        <v>336</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -1808,34 +1976,34 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F9" s="5">
         <v>13</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>171</v>
+        <v>335</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -1847,22 +2015,22 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F10" s="5">
         <v>5</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>19</v>
@@ -1871,10 +2039,10 @@
         <v>18</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>228</v>
+        <v>334</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="N10" s="4"/>
     </row>
@@ -1887,31 +2055,31 @@
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="5" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F11" s="5">
         <v>7</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>21</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>228</v>
+        <v>341</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="N11" s="4"/>
     </row>
@@ -1924,32 +2092,32 @@
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F12" s="4">
         <v>9</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>108</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>21</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>320</v>
+        <v>345</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="N12" s="4"/>
     </row>
@@ -1962,33 +2130,35 @@
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="5" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F13" s="5">
         <v>7</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>21</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>228</v>
+        <v>341</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>316</v>
-      </c>
-      <c r="N13" s="4"/>
+        <v>312</v>
+      </c>
+      <c r="N13" s="4" t="s">
+        <v>342</v>
+      </c>
     </row>
     <row r="14" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="5">
@@ -1998,20 +2168,20 @@
         <v>152</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F14" s="5">
         <v>10</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>108</v>
@@ -2020,10 +2190,10 @@
         <v>23</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="N14" s="4"/>
     </row>
@@ -2036,31 +2206,31 @@
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="5" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F15" s="5">
         <v>8</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>228</v>
+        <v>340</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="N15" s="4"/>
     </row>
@@ -2074,7 +2244,7 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F16" s="4">
         <v>9</v>
@@ -2090,7 +2260,7 @@
         <v>18</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>229</v>
+        <v>332</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>22</v>
@@ -2107,7 +2277,7 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F17" s="4">
         <v>10</v>
@@ -2123,7 +2293,7 @@
         <v>18</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>22</v>
@@ -2142,28 +2312,28 @@
         <v>11</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F18" s="4">
         <v>7</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>228</v>
+        <v>343</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="N18" s="4"/>
     </row>
@@ -2177,7 +2347,7 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F19" s="4">
         <v>10</v>
@@ -2193,14 +2363,14 @@
         <v>25</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>22</v>
       </c>
       <c r="N19" s="4"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="4">
         <v>17</v>
       </c>
@@ -2210,7 +2380,7 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F20" s="4">
         <v>9</v>
@@ -2226,7 +2396,7 @@
         <v>13</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>229</v>
+        <v>344</v>
       </c>
       <c r="M20" s="4" t="s">
         <v>22</v>
@@ -2243,7 +2413,7 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F21" s="4">
         <v>10</v>
@@ -2259,7 +2429,7 @@
         <v>23</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>229</v>
+        <v>331</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>22</v>
@@ -2276,7 +2446,7 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F22" s="4">
         <v>6</v>
@@ -2292,7 +2462,7 @@
         <v>13</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>22</v>
@@ -2319,7 +2489,7 @@
         <v>28</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>10</v>
@@ -2331,10 +2501,10 @@
         <v>29</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>228</v>
+        <v>330</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="N23" s="4"/>
     </row>
@@ -2366,10 +2536,10 @@
         <v>30</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>31</v>
@@ -2401,10 +2571,10 @@
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>31</v>
@@ -2436,10 +2606,10 @@
       </c>
       <c r="K26" s="4"/>
       <c r="L26" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N26" s="4" t="s">
         <v>31</v>
@@ -2471,10 +2641,10 @@
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>31</v>
@@ -2508,10 +2678,10 @@
         <v>32</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>31</v>
@@ -2545,10 +2715,10 @@
         <v>33</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>31</v>
@@ -2573,12 +2743,12 @@
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="1" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="N30" s="4"/>
     </row>
@@ -2600,22 +2770,22 @@
         <v>2</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="N31" s="4"/>
     </row>
@@ -2644,16 +2814,16 @@
         <v>113</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>36</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="N32" s="4"/>
     </row>
@@ -2685,10 +2855,10 @@
         <v>24</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="N33" s="4"/>
     </row>
@@ -2717,14 +2887,14 @@
         <v>115</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="80" x14ac:dyDescent="0.2">
@@ -2754,10 +2924,10 @@
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="80" x14ac:dyDescent="0.2">
@@ -2785,14 +2955,14 @@
         <v>38</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="L36" s="4"/>
       <c r="M36" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -2856,10 +3026,10 @@
         <v>41</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="N38" s="4" t="s">
         <v>31</v>
@@ -2891,10 +3061,10 @@
       </c>
       <c r="K39" s="4"/>
       <c r="L39" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="N39" s="4" t="s">
         <v>31</v>
@@ -2926,10 +3096,10 @@
       </c>
       <c r="K40" s="4"/>
       <c r="L40" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="N40" s="4" t="s">
         <v>31</v>
@@ -2961,10 +3131,10 @@
       </c>
       <c r="K41" s="4"/>
       <c r="L41" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="N41" s="4" t="s">
         <v>31</v>
@@ -2995,13 +3165,13 @@
         <v>111</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="N42" s="4"/>
     </row>
@@ -3033,10 +3203,10 @@
         <v>43</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="N43" s="4"/>
     </row>
@@ -3067,7 +3237,7 @@
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
       <c r="M44" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N44" s="4"/>
     </row>
@@ -3097,10 +3267,10 @@
       </c>
       <c r="K45" s="4"/>
       <c r="L45" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>31</v>
@@ -3132,10 +3302,10 @@
       </c>
       <c r="K46" s="4"/>
       <c r="L46" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="N46" s="4"/>
     </row>
@@ -3151,28 +3321,28 @@
         <v>44</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F47" s="4">
         <v>10</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="K47" s="4" t="s">
         <v>44</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="N47" s="4"/>
     </row>
@@ -3188,7 +3358,7 @@
         <v>43</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F48" s="4">
         <v>14</v>
@@ -3204,10 +3374,10 @@
         <v>32</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N48" s="4"/>
     </row>
@@ -3223,7 +3393,7 @@
         <v>42</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F49" s="4">
         <v>8</v>
@@ -3239,10 +3409,10 @@
         <v>45</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="N49" s="4"/>
     </row>
@@ -3264,22 +3434,22 @@
         <v>17</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I50" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="K50" s="4" t="s">
         <v>182</v>
       </c>
-      <c r="K50" s="4" t="s">
-        <v>183</v>
-      </c>
       <c r="L50" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>31</v>
@@ -3303,22 +3473,22 @@
         <v>17</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="K51" s="4" t="s">
         <v>47</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>31</v>
@@ -3333,16 +3503,16 @@
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F52" s="4">
         <v>12</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>10</v>
@@ -3351,16 +3521,16 @@
         <v>48</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="K52" s="4" t="s">
         <v>20</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="N52" s="4"/>
     </row>
@@ -3390,10 +3560,10 @@
         <v>50</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="N53" s="4" t="s">
         <v>51</v>
@@ -3417,7 +3587,7 @@
         <v>14</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>10</v>
@@ -3429,10 +3599,10 @@
         <v>54</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>228</v>
+        <v>333</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="N54" s="4"/>
     </row>
@@ -3452,22 +3622,22 @@
         <v>7</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="K55" s="4" t="s">
         <v>55</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="N55" s="4"/>
     </row>
@@ -3487,7 +3657,7 @@
         <v>12</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="H56" s="4" t="s">
         <v>61</v>
@@ -3497,10 +3667,10 @@
       </c>
       <c r="K56" s="4"/>
       <c r="L56" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="N56" s="4"/>
     </row>
@@ -3522,7 +3692,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H57" s="4" t="s">
         <v>61</v>
@@ -3534,10 +3704,10 @@
         <v>58</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="N57" s="4"/>
     </row>
@@ -3568,7 +3738,7 @@
       </c>
       <c r="L58" s="4"/>
       <c r="M58" s="5" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="N58" s="4"/>
     </row>
@@ -3596,10 +3766,10 @@
       </c>
       <c r="K59" s="4"/>
       <c r="L59" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M59" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="N59" s="4"/>
     </row>
@@ -3629,10 +3799,10 @@
         <v>65</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M60" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="N60" s="4"/>
     </row>
@@ -3648,26 +3818,26 @@
         <v>10</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F61" s="4">
         <v>6</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="H61" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="K61" s="4"/>
       <c r="L61" s="4" t="s">
-        <v>228</v>
+        <v>343</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N61" s="4"/>
     </row>
@@ -3699,10 +3869,10 @@
         <v>67</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="M62" s="4" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="N62" s="4"/>
     </row>
@@ -3734,10 +3904,10 @@
         <v>69</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="N63" s="4"/>
     </row>
@@ -3769,10 +3939,10 @@
         <v>70</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="N64" s="4"/>
     </row>
@@ -3800,10 +3970,10 @@
       </c>
       <c r="K65" s="4"/>
       <c r="L65" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="N65" s="4"/>
     </row>
@@ -3833,10 +4003,10 @@
         <v>72</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="N66" s="4"/>
     </row>
@@ -3868,10 +4038,10 @@
         <v>73</v>
       </c>
       <c r="L67" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="N67" s="4"/>
     </row>
@@ -3893,7 +4063,7 @@
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
       <c r="I68" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="J68" s="1" t="s">
         <v>75</v>
@@ -3901,7 +4071,7 @@
       <c r="K68" s="4"/>
       <c r="L68" s="4"/>
       <c r="M68" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N68" s="4"/>
     </row>
@@ -3928,7 +4098,7 @@
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
       <c r="M69" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="N69" s="4"/>
     </row>
@@ -3955,7 +4125,7 @@
       <c r="K70" s="4"/>
       <c r="L70" s="4"/>
       <c r="M70" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="N70" s="4"/>
     </row>
@@ -3975,7 +4145,7 @@
         <v>5</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H71" s="4" t="s">
         <v>10</v>
@@ -3987,10 +4157,10 @@
         <v>76</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="N71" s="4"/>
     </row>
@@ -4018,10 +4188,10 @@
         <v>77</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M72" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="N72" s="4"/>
     </row>
@@ -4051,10 +4221,10 @@
         <v>78</v>
       </c>
       <c r="L73" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M73" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="N73" s="4"/>
     </row>
@@ -4084,10 +4254,10 @@
         <v>79</v>
       </c>
       <c r="L74" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M74" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="N74" s="4"/>
     </row>
@@ -4117,10 +4287,10 @@
         <v>79</v>
       </c>
       <c r="L75" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M75" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="N75" s="4"/>
     </row>
@@ -4150,10 +4320,10 @@
         <v>79</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="N76" s="4"/>
     </row>
@@ -4185,10 +4355,10 @@
         <v>81</v>
       </c>
       <c r="L77" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M77" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="N77" s="4"/>
     </row>
@@ -4218,10 +4388,10 @@
         <v>82</v>
       </c>
       <c r="L78" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M78" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="N78" s="4"/>
     </row>
@@ -4251,10 +4421,10 @@
         <v>83</v>
       </c>
       <c r="L79" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M79" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="N79" s="4"/>
     </row>
@@ -4276,7 +4446,7 @@
         <v>5</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="H80" s="4" t="s">
         <v>61</v>
@@ -4286,13 +4456,13 @@
       </c>
       <c r="K80" s="4"/>
       <c r="L80" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M80" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N80" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -4320,7 +4490,7 @@
       </c>
       <c r="L81" s="4"/>
       <c r="M81" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="N81" s="4"/>
     </row>
@@ -4336,7 +4506,7 @@
         <v>48</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F82" s="4">
         <v>3</v>
@@ -4350,10 +4520,10 @@
         <v>85</v>
       </c>
       <c r="L82" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M82" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N82" s="4" t="s">
         <v>31</v>
@@ -4377,20 +4547,20 @@
         <v>2</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="H83" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="K83" s="4" t="s">
         <v>87</v>
       </c>
       <c r="L83" s="4"/>
       <c r="M83" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="N83" s="4"/>
     </row>
@@ -4412,7 +4582,7 @@
         <v>1</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="H84" s="4" t="s">
         <v>10</v>
@@ -4425,7 +4595,7 @@
       </c>
       <c r="L84" s="4"/>
       <c r="M84" s="4" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="N84" s="4"/>
     </row>
@@ -4454,16 +4624,16 @@
         <v>139</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="K85" s="4" t="s">
         <v>91</v>
       </c>
       <c r="L85" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="M85" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="N85" s="4"/>
     </row>
@@ -4495,10 +4665,10 @@
         <v>92</v>
       </c>
       <c r="L86" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="M86" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="N86" s="4"/>
     </row>
@@ -4528,10 +4698,10 @@
         <v>94</v>
       </c>
       <c r="L87" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M87" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="N87" s="4" t="s">
         <v>26</v>
@@ -4560,7 +4730,7 @@
       <c r="K88" s="4"/>
       <c r="L88" s="4"/>
       <c r="M88" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N88" s="4"/>
     </row>
@@ -4587,7 +4757,7 @@
       <c r="K89" s="4"/>
       <c r="L89" s="4"/>
       <c r="M89" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N89" s="4"/>
     </row>
@@ -4614,7 +4784,7 @@
       <c r="K90" s="4"/>
       <c r="L90" s="4"/>
       <c r="M90" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N90" s="4" t="s">
         <v>99</v>
@@ -4643,7 +4813,7 @@
       <c r="K91" s="4"/>
       <c r="L91" s="4"/>
       <c r="M91" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N91" s="4" t="s">
         <v>99</v>
@@ -4672,7 +4842,7 @@
       <c r="K92" s="4"/>
       <c r="L92" s="4"/>
       <c r="M92" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N92" s="4" t="s">
         <v>99</v>
@@ -4699,7 +4869,7 @@
       <c r="K93" s="4"/>
       <c r="L93" s="4"/>
       <c r="M93" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N93" s="4" t="s">
         <v>99</v>
@@ -4726,7 +4896,7 @@
       <c r="K94" s="4"/>
       <c r="L94" s="4"/>
       <c r="M94" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N94" s="4" t="s">
         <v>99</v>
@@ -4755,7 +4925,7 @@
       <c r="K95" s="4"/>
       <c r="L95" s="4"/>
       <c r="M95" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N95" s="4" t="s">
         <v>31</v>
@@ -4809,7 +4979,7 @@
       <c r="K97" s="4"/>
       <c r="L97" s="4"/>
       <c r="M97" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N97" s="4"/>
     </row>
@@ -4834,7 +5004,7 @@
       <c r="K98" s="4"/>
       <c r="L98" s="4"/>
       <c r="M98" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="N98" s="4" t="s">
         <v>31</v>
@@ -4869,7 +5039,7 @@
       </c>
       <c r="L99" s="4"/>
       <c r="M99" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N99" s="4"/>
     </row>
@@ -4898,16 +5068,16 @@
         <v>147</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="K100" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L100" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M100" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="N100" s="4"/>
     </row>
@@ -4936,16 +5106,16 @@
         <v>104</v>
       </c>
       <c r="J101" s="7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="K101" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="L101" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M101" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="N101" s="4"/>
     </row>
@@ -4974,14 +5144,14 @@
         <v>104</v>
       </c>
       <c r="J102" s="7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="K102" s="4"/>
       <c r="L102" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M102" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="N102" s="4"/>
     </row>
@@ -5008,14 +5178,14 @@
         <v>104</v>
       </c>
       <c r="J103" s="7" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="K103" s="4"/>
       <c r="L103" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M103" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="N103" s="4" t="s">
         <v>31</v>
@@ -5043,7 +5213,7 @@
       </c>
       <c r="K104" s="4"/>
       <c r="L104" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M104" s="4" t="s">
         <v>22</v>
@@ -5060,7 +5230,7 @@
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
       <c r="E105" s="4" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="F105" s="4">
         <v>6</v>
@@ -5072,7 +5242,7 @@
       </c>
       <c r="K105" s="4"/>
       <c r="L105" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M105" s="4" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
edits to text files, adds to Library, edits to inventory
</commit_message>
<xml_diff>
--- a/metadata/Inventory_Iksvaku.xlsx
+++ b/metadata/Inventory_Iksvaku.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="4660" windowWidth="25480" windowHeight="9100" tabRatio="500"/>
+    <workbookView xWindow="280" yWindow="2460" windowWidth="25480" windowHeight="9100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="364">
   <si>
     <t>(Faces:) Lines</t>
   </si>
@@ -514,9 +514,6 @@
   </si>
   <si>
     <t>13C</t>
-  </si>
-  <si>
-    <t>13D</t>
   </si>
   <si>
     <t>12A</t>
@@ -661,9 +658,6 @@
     <t>Vogel, Additional Prakrit Inscriptions from Nagarjunakonda, M1 (EI Vol. XXI, p. 65f., plate M-1)</t>
   </si>
   <si>
-    <t>Sarkar (EI Vol. XXXVIII, p. 177, M21)</t>
-  </si>
-  <si>
     <t>Vogel M9 (EI Vol. XXI, p. 67, plate M-9)</t>
   </si>
   <si>
@@ -758,9 +752,6 @@
   </si>
   <si>
     <t>Chhabra (EI Vol. XXXIII, p. 149, No. 27)</t>
-  </si>
-  <si>
-    <t>Sarkar (EI Vol. XXXVIII, pt. IV, pp. 177)</t>
   </si>
   <si>
     <t>Sircar (EI Vol. XXXIV, pt. I, pp. 17-20)</t>
@@ -1064,48 +1055,6 @@
   </si>
   <si>
     <t>No rubbing for our IKS006 in Raghunath. See remark under IKS005.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Corps)"/>
-      </rPr>
-      <t>estampage Leiden N10. —</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Vogel; Raghunath</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Corps)"/>
-      </rPr>
-      <t>estampage Leiden N15. —</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Raghunath</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1246,12 +1195,147 @@
       <t>Sankaranarayanan 1969-70: 317-8. — Raghunath 2001: 70-1 (3).</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve"> east side of the Mahācaitya, Nāgārjunakoṇḍa Site-1</t>
+  </si>
+  <si>
+    <t>estampage Leiden N15 (three separate sheets).</t>
+  </si>
+  <si>
+    <t>south of the Mahācaitya at Nāgārjunakoṇḍa Site-1</t>
+  </si>
+  <si>
+    <t>estampage Leiden N9.</t>
+  </si>
+  <si>
+    <t>13D, 24</t>
+  </si>
+  <si>
+    <t>Naga 39</t>
+  </si>
+  <si>
+    <t>Raghunath assigns wto separates entries to a single item.</t>
+  </si>
+  <si>
+    <t>Sarkar 1969: 177 (M21). — Raghunath 2001: 110, 127.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Corps)"/>
+      </rPr>
+      <t>estampage Leiden N10 (two separate sheets). —</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Vogel; Raghunath</t>
+    </r>
+  </si>
+  <si>
+    <t>Raghunath's plate is inverted horizontally.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Corps)"/>
+      </rPr>
+      <t>estampage Leiden N15 (two sheets). —</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Raghunath</t>
+    </r>
+  </si>
+  <si>
+    <t>Sanskrit and MIA</t>
+  </si>
+  <si>
+    <t>Phanigiri</t>
+  </si>
+  <si>
+    <t>storage center in village</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Corps)"/>
+      </rPr>
+      <t>IAR 2002–03; 2003–04. — Munirathnam 2005. — Subrahmanyam &amp; Reddy 2008. —</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="136"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Ramesh &amp; Muniratnam 2011. — </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Skilling &amp; von Hinüber 2011.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Corps)"/>
+      </rPr>
+      <t xml:space="preserve">IAR 2002–03; 2003–04. — Munirathnam 2005. — Subrahmanyam &amp; Reddy 2008. — </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>von Hinüber 2012; 2013.</t>
+    </r>
+  </si>
+  <si>
+    <t>other Phanigiri</t>
+  </si>
+  <si>
+    <t>Guntupalle</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1301,6 +1385,11 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri (Corps)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri (Corps)"/>
     </font>
   </fonts>
@@ -1689,10 +1778,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N106"/>
+  <dimension ref="A1:N113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="83" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="83" workbookViewId="0">
+      <selection activeCell="A114" sqref="A114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1715,26 +1804,26 @@
   <sheetData>
     <row r="1" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="E2" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>9</v>
@@ -1783,10 +1872,10 @@
         <v>4</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>11</v>
@@ -1798,10 +1887,10 @@
         <v>13</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="N4" s="4"/>
     </row>
@@ -1816,7 +1905,7 @@
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>107</v>
@@ -1825,28 +1914,28 @@
         <v>15</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H5" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>298</v>
-      </c>
       <c r="J5" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="K5" s="4" t="s">
-        <v>300</v>
-      </c>
       <c r="L5" s="5" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="112" x14ac:dyDescent="0.2">
@@ -1858,7 +1947,7 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>15</v>
@@ -1867,25 +1956,25 @@
         <v>4</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="N6" s="4"/>
     </row>
@@ -1901,31 +1990,31 @@
         <v>1</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F7" s="5">
         <v>13</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="K7" s="4" t="s">
         <v>17</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="64" x14ac:dyDescent="0.2">
@@ -1937,34 +2026,34 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="5" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F8" s="5">
         <v>12</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="K8" s="4" t="s">
         <v>20</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -1976,34 +2065,34 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F9" s="5">
         <v>13</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="K9" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>335</v>
+        <v>330</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -2015,22 +2104,22 @@
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F10" s="5">
         <v>5</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>19</v>
@@ -2039,10 +2128,10 @@
         <v>18</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>334</v>
+        <v>329</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="N10" s="4"/>
     </row>
@@ -2055,31 +2144,31 @@
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="5" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F11" s="5">
         <v>7</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>21</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="N11" s="4"/>
     </row>
@@ -2092,32 +2181,32 @@
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F12" s="4">
         <v>9</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>108</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>21</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="N12" s="4"/>
     </row>
@@ -2130,34 +2219,34 @@
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="5" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F13" s="5">
         <v>7</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="K13" s="4" t="s">
         <v>21</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -2168,20 +2257,20 @@
         <v>152</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F14" s="5">
         <v>10</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>108</v>
@@ -2190,10 +2279,10 @@
         <v>23</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="N14" s="4"/>
     </row>
@@ -2206,31 +2295,31 @@
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="5" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F15" s="5">
         <v>8</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="K15" s="4" t="s">
         <v>24</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="N15" s="4"/>
     </row>
@@ -2244,7 +2333,7 @@
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F16" s="4">
         <v>9</v>
@@ -2260,7 +2349,7 @@
         <v>18</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="M16" s="4" t="s">
         <v>22</v>
@@ -2277,7 +2366,7 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F17" s="4">
         <v>10</v>
@@ -2293,7 +2382,7 @@
         <v>18</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M17" s="4" t="s">
         <v>22</v>
@@ -2312,28 +2401,28 @@
         <v>11</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F18" s="4">
         <v>7</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="K18" s="4" t="s">
         <v>18</v>
       </c>
       <c r="L18" s="4" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="M18" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="N18" s="4"/>
     </row>
@@ -2347,7 +2436,7 @@
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F19" s="4">
         <v>10</v>
@@ -2363,7 +2452,7 @@
         <v>25</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M19" s="4" t="s">
         <v>22</v>
@@ -2380,7 +2469,7 @@
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F20" s="4">
         <v>9</v>
@@ -2396,7 +2485,7 @@
         <v>13</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="M20" s="4" t="s">
         <v>22</v>
@@ -2413,7 +2502,7 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F21" s="4">
         <v>10</v>
@@ -2429,7 +2518,7 @@
         <v>23</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>331</v>
+        <v>356</v>
       </c>
       <c r="M21" s="4" t="s">
         <v>22</v>
@@ -2446,7 +2535,7 @@
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F22" s="4">
         <v>6</v>
@@ -2462,7 +2551,7 @@
         <v>13</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M22" s="4" t="s">
         <v>22</v>
@@ -2489,7 +2578,7 @@
         <v>28</v>
       </c>
       <c r="G23" s="4" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="H23" s="4" t="s">
         <v>10</v>
@@ -2501,10 +2590,10 @@
         <v>29</v>
       </c>
       <c r="L23" s="4" t="s">
-        <v>330</v>
+        <v>354</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="N23" s="4"/>
     </row>
@@ -2536,10 +2625,10 @@
         <v>30</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N24" s="4" t="s">
         <v>31</v>
@@ -2550,7 +2639,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4">
@@ -2571,10 +2660,10 @@
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>31</v>
@@ -2585,7 +2674,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4">
@@ -2606,10 +2695,10 @@
       </c>
       <c r="K26" s="4"/>
       <c r="L26" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="N26" s="4" t="s">
         <v>31</v>
@@ -2641,10 +2730,10 @@
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N27" s="4" t="s">
         <v>31</v>
@@ -2678,10 +2767,10 @@
         <v>32</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>31</v>
@@ -2715,24 +2804,26 @@
         <v>33</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A30" s="4">
         <v>27</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>162</v>
+        <v>350</v>
       </c>
       <c r="C30" s="4"/>
-      <c r="D30" s="4"/>
+      <c r="D30" s="4" t="s">
+        <v>351</v>
+      </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4">
         <v>3</v>
@@ -2741,16 +2832,20 @@
       <c r="H30" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I30" s="4"/>
+      <c r="I30" s="4" t="s">
+        <v>111</v>
+      </c>
       <c r="J30" s="1" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4" t="s">
-        <v>235</v>
-      </c>
-      <c r="N30" s="4"/>
+        <v>353</v>
+      </c>
+      <c r="N30" s="4" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="31" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A31" s="4">
@@ -2770,22 +2865,22 @@
         <v>2</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="N31" s="4"/>
     </row>
@@ -2814,16 +2909,16 @@
         <v>113</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>36</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="N32" s="4"/>
     </row>
@@ -2855,10 +2950,10 @@
         <v>24</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="N33" s="4"/>
     </row>
@@ -2867,7 +2962,7 @@
         <v>31</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4">
@@ -2887,14 +2982,14 @@
         <v>115</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="80" x14ac:dyDescent="0.2">
@@ -2924,10 +3019,10 @@
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="80" x14ac:dyDescent="0.2">
@@ -2935,7 +3030,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4">
@@ -2955,14 +3050,14 @@
         <v>38</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="L36" s="4"/>
       <c r="M36" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3003,7 +3098,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4">
@@ -3026,10 +3121,10 @@
         <v>41</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="N38" s="4" t="s">
         <v>31</v>
@@ -3061,10 +3156,10 @@
       </c>
       <c r="K39" s="4"/>
       <c r="L39" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N39" s="4" t="s">
         <v>31</v>
@@ -3096,10 +3191,10 @@
       </c>
       <c r="K40" s="4"/>
       <c r="L40" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="N40" s="4" t="s">
         <v>31</v>
@@ -3131,10 +3226,10 @@
       </c>
       <c r="K41" s="4"/>
       <c r="L41" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="N41" s="4" t="s">
         <v>31</v>
@@ -3165,13 +3260,13 @@
         <v>111</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="N42" s="4"/>
     </row>
@@ -3203,23 +3298,23 @@
         <v>43</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="N43" s="4"/>
     </row>
-    <row r="44" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A44" s="4">
         <v>41</v>
       </c>
-      <c r="B44" s="4">
-        <v>24</v>
+      <c r="B44" s="4" t="s">
+        <v>312</v>
       </c>
       <c r="C44" s="4"/>
-      <c r="D44" s="4">
-        <v>39</v>
+      <c r="D44" s="4" t="s">
+        <v>312</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>12</v>
@@ -3229,15 +3324,13 @@
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>111</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="I44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
       <c r="M44" s="4" t="s">
-        <v>202</v>
+        <v>22</v>
       </c>
       <c r="N44" s="4"/>
     </row>
@@ -3267,10 +3360,10 @@
       </c>
       <c r="K45" s="4"/>
       <c r="L45" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>31</v>
@@ -3302,10 +3395,10 @@
       </c>
       <c r="K46" s="4"/>
       <c r="L46" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="N46" s="4"/>
     </row>
@@ -3321,28 +3414,28 @@
         <v>44</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F47" s="4">
         <v>10</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="K47" s="4" t="s">
         <v>44</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="N47" s="4"/>
     </row>
@@ -3358,7 +3451,7 @@
         <v>43</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F48" s="4">
         <v>14</v>
@@ -3374,10 +3467,10 @@
         <v>32</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="N48" s="4"/>
     </row>
@@ -3393,7 +3486,7 @@
         <v>42</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="F49" s="4">
         <v>8</v>
@@ -3409,10 +3502,10 @@
         <v>45</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="N49" s="4"/>
     </row>
@@ -3434,22 +3527,22 @@
         <v>17</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I50" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="K50" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="K50" s="4" t="s">
-        <v>182</v>
-      </c>
       <c r="L50" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="N50" s="4" t="s">
         <v>31</v>
@@ -3473,22 +3566,22 @@
         <v>17</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="K51" s="4" t="s">
         <v>47</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>31</v>
@@ -3503,16 +3596,16 @@
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F52" s="4">
         <v>12</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>10</v>
@@ -3521,16 +3614,16 @@
         <v>48</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="K52" s="4" t="s">
         <v>20</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="N52" s="4"/>
     </row>
@@ -3560,10 +3653,10 @@
         <v>50</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="N53" s="4" t="s">
         <v>51</v>
@@ -3587,7 +3680,7 @@
         <v>14</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>10</v>
@@ -3599,12 +3692,14 @@
         <v>54</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>333</v>
+        <v>328</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="N54" s="4"/>
+        <v>208</v>
+      </c>
+      <c r="N54" s="4" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="55" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A55" s="4">
@@ -3622,22 +3717,22 @@
         <v>7</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="K55" s="4" t="s">
         <v>55</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="N55" s="4"/>
     </row>
@@ -3657,7 +3752,7 @@
         <v>12</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="H56" s="4" t="s">
         <v>61</v>
@@ -3667,10 +3762,10 @@
       </c>
       <c r="K56" s="4"/>
       <c r="L56" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M56" s="4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="N56" s="4"/>
     </row>
@@ -3692,7 +3787,7 @@
         <v>1</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="H57" s="4" t="s">
         <v>61</v>
@@ -3704,10 +3799,10 @@
         <v>58</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="N57" s="4"/>
     </row>
@@ -3716,7 +3811,7 @@
         <v>55</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
@@ -3738,7 +3833,7 @@
       </c>
       <c r="L58" s="4"/>
       <c r="M58" s="5" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="N58" s="4"/>
     </row>
@@ -3766,10 +3861,10 @@
       </c>
       <c r="K59" s="4"/>
       <c r="L59" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M59" s="4" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="N59" s="4"/>
     </row>
@@ -3799,10 +3894,10 @@
         <v>65</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M60" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="N60" s="4"/>
     </row>
@@ -3818,26 +3913,26 @@
         <v>10</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F61" s="4">
         <v>6</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="H61" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="K61" s="4"/>
       <c r="L61" s="4" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="N61" s="4"/>
     </row>
@@ -3869,10 +3964,10 @@
         <v>67</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M62" s="4" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="N62" s="4"/>
     </row>
@@ -3904,10 +3999,10 @@
         <v>69</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="N63" s="4"/>
     </row>
@@ -3939,10 +4034,10 @@
         <v>70</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N64" s="4"/>
     </row>
@@ -3970,10 +4065,10 @@
       </c>
       <c r="K65" s="4"/>
       <c r="L65" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="N65" s="4"/>
     </row>
@@ -4003,10 +4098,10 @@
         <v>72</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="N66" s="4"/>
     </row>
@@ -4038,10 +4133,10 @@
         <v>73</v>
       </c>
       <c r="L67" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="N67" s="4"/>
     </row>
@@ -4063,7 +4158,7 @@
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
       <c r="I68" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="J68" s="1" t="s">
         <v>75</v>
@@ -4071,7 +4166,7 @@
       <c r="K68" s="4"/>
       <c r="L68" s="4"/>
       <c r="M68" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N68" s="4"/>
     </row>
@@ -4098,7 +4193,7 @@
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
       <c r="M69" s="4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="N69" s="4"/>
     </row>
@@ -4125,7 +4220,7 @@
       <c r="K70" s="4"/>
       <c r="L70" s="4"/>
       <c r="M70" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="N70" s="4"/>
     </row>
@@ -4145,7 +4240,7 @@
         <v>5</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="H71" s="4" t="s">
         <v>10</v>
@@ -4157,10 +4252,10 @@
         <v>76</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="N71" s="4"/>
     </row>
@@ -4188,10 +4283,10 @@
         <v>77</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M72" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="N72" s="4"/>
     </row>
@@ -4221,10 +4316,10 @@
         <v>78</v>
       </c>
       <c r="L73" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M73" s="4" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="N73" s="4"/>
     </row>
@@ -4254,10 +4349,10 @@
         <v>79</v>
       </c>
       <c r="L74" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M74" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="N74" s="4"/>
     </row>
@@ -4287,10 +4382,10 @@
         <v>79</v>
       </c>
       <c r="L75" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M75" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="N75" s="4"/>
     </row>
@@ -4320,10 +4415,10 @@
         <v>79</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="N76" s="4"/>
     </row>
@@ -4355,10 +4450,10 @@
         <v>81</v>
       </c>
       <c r="L77" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M77" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="N77" s="4"/>
     </row>
@@ -4388,10 +4483,10 @@
         <v>82</v>
       </c>
       <c r="L78" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M78" s="4" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="N78" s="4"/>
     </row>
@@ -4421,10 +4516,10 @@
         <v>83</v>
       </c>
       <c r="L79" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M79" s="4" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="N79" s="4"/>
     </row>
@@ -4446,7 +4541,7 @@
         <v>5</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="H80" s="4" t="s">
         <v>61</v>
@@ -4456,13 +4551,13 @@
       </c>
       <c r="K80" s="4"/>
       <c r="L80" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="M80" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="N80" s="4" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -4470,7 +4565,7 @@
         <v>78</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
@@ -4490,7 +4585,7 @@
       </c>
       <c r="L81" s="4"/>
       <c r="M81" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="N81" s="4"/>
     </row>
@@ -4506,7 +4601,7 @@
         <v>48</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F82" s="4">
         <v>3</v>
@@ -4520,10 +4615,10 @@
         <v>85</v>
       </c>
       <c r="L82" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M82" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="N82" s="4" t="s">
         <v>31</v>
@@ -4547,20 +4642,20 @@
         <v>2</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="H83" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="K83" s="4" t="s">
         <v>87</v>
       </c>
       <c r="L83" s="4"/>
       <c r="M83" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="N83" s="4"/>
     </row>
@@ -4582,7 +4677,7 @@
         <v>1</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="H84" s="4" t="s">
         <v>10</v>
@@ -4595,7 +4690,7 @@
       </c>
       <c r="L84" s="4"/>
       <c r="M84" s="4" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="N84" s="4"/>
     </row>
@@ -4624,16 +4719,16 @@
         <v>139</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="K85" s="4" t="s">
         <v>91</v>
       </c>
       <c r="L85" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="M85" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N85" s="4"/>
     </row>
@@ -4665,10 +4760,10 @@
         <v>92</v>
       </c>
       <c r="L86" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M86" s="4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="N86" s="4"/>
     </row>
@@ -4698,10 +4793,10 @@
         <v>94</v>
       </c>
       <c r="L87" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M87" s="4" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="N87" s="4" t="s">
         <v>26</v>
@@ -4730,7 +4825,7 @@
       <c r="K88" s="4"/>
       <c r="L88" s="4"/>
       <c r="M88" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N88" s="4"/>
     </row>
@@ -4757,7 +4852,7 @@
       <c r="K89" s="4"/>
       <c r="L89" s="4"/>
       <c r="M89" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N89" s="4"/>
     </row>
@@ -4784,7 +4879,7 @@
       <c r="K90" s="4"/>
       <c r="L90" s="4"/>
       <c r="M90" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N90" s="4" t="s">
         <v>99</v>
@@ -4813,7 +4908,7 @@
       <c r="K91" s="4"/>
       <c r="L91" s="4"/>
       <c r="M91" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N91" s="4" t="s">
         <v>99</v>
@@ -4842,7 +4937,7 @@
       <c r="K92" s="4"/>
       <c r="L92" s="4"/>
       <c r="M92" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N92" s="4" t="s">
         <v>99</v>
@@ -4869,7 +4964,7 @@
       <c r="K93" s="4"/>
       <c r="L93" s="4"/>
       <c r="M93" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N93" s="4" t="s">
         <v>99</v>
@@ -4896,7 +4991,7 @@
       <c r="K94" s="4"/>
       <c r="L94" s="4"/>
       <c r="M94" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N94" s="4" t="s">
         <v>99</v>
@@ -4925,7 +5020,7 @@
       <c r="K95" s="4"/>
       <c r="L95" s="4"/>
       <c r="M95" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N95" s="4" t="s">
         <v>31</v>
@@ -4979,7 +5074,7 @@
       <c r="K97" s="4"/>
       <c r="L97" s="4"/>
       <c r="M97" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N97" s="4"/>
     </row>
@@ -5004,7 +5099,7 @@
       <c r="K98" s="4"/>
       <c r="L98" s="4"/>
       <c r="M98" s="4" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="N98" s="4" t="s">
         <v>31</v>
@@ -5039,7 +5134,7 @@
       </c>
       <c r="L99" s="4"/>
       <c r="M99" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="N99" s="4"/>
     </row>
@@ -5068,16 +5163,16 @@
         <v>147</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="K100" s="4" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L100" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M100" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="N100" s="4"/>
     </row>
@@ -5106,16 +5201,16 @@
         <v>104</v>
       </c>
       <c r="J101" s="7" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="K101" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="L101" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M101" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="N101" s="4"/>
     </row>
@@ -5144,14 +5239,14 @@
         <v>104</v>
       </c>
       <c r="J102" s="7" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="K102" s="4"/>
       <c r="L102" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M102" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="N102" s="4"/>
     </row>
@@ -5178,14 +5273,14 @@
         <v>104</v>
       </c>
       <c r="J103" s="7" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="K103" s="4"/>
       <c r="L103" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M103" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="N103" s="4" t="s">
         <v>31</v>
@@ -5213,7 +5308,7 @@
       </c>
       <c r="K104" s="4"/>
       <c r="L104" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M104" s="4" t="s">
         <v>22</v>
@@ -5230,7 +5325,7 @@
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
       <c r="E105" s="4" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="F105" s="4">
         <v>6</v>
@@ -5242,7 +5337,7 @@
       </c>
       <c r="K105" s="4"/>
       <c r="L105" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M105" s="4" t="s">
         <v>22</v>
@@ -5273,6 +5368,167 @@
       <c r="L106" s="4"/>
       <c r="M106" s="4"/>
       <c r="N106" s="4"/>
+    </row>
+    <row r="107" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>104</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F107" s="1">
+        <v>11</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L107" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="M107" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="108" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>105</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F108" s="1">
+        <v>10</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L108" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="M108" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <v>106</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="F109" s="1">
+        <v>10</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="L109" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="M109" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" ht="80" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <v>107</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F110" s="1">
+        <v>10</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="J110" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="M110" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <v>108</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F111" s="1">
+        <v>20</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="M111" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A112" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A113" s="1" t="s">
+        <v>363</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
edits to text file and inventory
</commit_message>
<xml_diff>
--- a/metadata/Inventory_Iksvaku.xlsx
+++ b/metadata/Inventory_Iksvaku.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="280" yWindow="2460" windowWidth="25480" windowHeight="9100" tabRatio="500"/>
+    <workbookView xWindow="120" yWindow="2460" windowWidth="25480" windowHeight="9100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="365">
   <si>
     <t>(Faces:) Lines</t>
   </si>
@@ -1305,6 +1305,15 @@
     </r>
   </si>
   <si>
+    <t>other Phanigiri</t>
+  </si>
+  <si>
+    <t>Guntupalle</t>
+  </si>
+  <si>
+    <t>Subrahmanyam &amp; Reddy 2008. — von Hinüber 2013.</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -1316,19 +1325,14 @@
     <r>
       <rPr>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="136"/>
         <scheme val="minor"/>
       </rPr>
       <t>von Hinüber 2012; 2013.</t>
     </r>
-  </si>
-  <si>
-    <t>other Phanigiri</t>
-  </si>
-  <si>
-    <t>Guntupalle</t>
   </si>
 </sst>
 </file>
@@ -1778,10 +1782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N113"/>
+  <dimension ref="A1:N116"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A110" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="83" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114"/>
+      <selection activeCell="M111" sqref="M111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5516,18 +5520,87 @@
       <c r="I111" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="M111" s="1" t="s">
+      <c r="M111" s="4" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="112" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <v>109</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F112" s="1">
+        <v>6</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="I112" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="M112" s="4" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <v>110</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F113" s="1">
+        <v>4</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="M113" s="4" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="114" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
+        <v>111</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="F114" s="1">
+        <v>3</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="I114" s="1" t="s">
+        <v>358</v>
+      </c>
+      <c r="M114" s="4" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A115" s="1" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="112" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A112" s="1" t="s">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A116" s="1" t="s">
         <v>362</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A113" s="1" t="s">
-        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edits to text file and to inventory, with shift of numbering IKS105>IKS014 now fully applied and high inv numbers shifted as a result
</commit_message>
<xml_diff>
--- a/metadata/Inventory_Iksvaku.xlsx
+++ b/metadata/Inventory_Iksvaku.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="2460" windowWidth="25480" windowHeight="9100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="9280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="369">
   <si>
     <t>(Faces:) Lines</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Kēsānapalli, Palnad Taluk, Guntur District</t>
   </si>
   <si>
-    <t>broken octogenal pillar</t>
-  </si>
-  <si>
     <t>erection of a Buddha statue</t>
   </si>
   <si>
@@ -99,9 +96,6 @@
   </si>
   <si>
     <t>erection of a pillar</t>
-  </si>
-  <si>
-    <t>ereection of a pillar for attaining bliss or nirvana</t>
   </si>
   <si>
     <t>incomplete</t>
@@ -483,16 +477,10 @@
     <t>6A</t>
   </si>
   <si>
-    <t>7A</t>
-  </si>
-  <si>
     <t>8A</t>
   </si>
   <si>
     <t>9A</t>
-  </si>
-  <si>
-    <t>9B</t>
   </si>
   <si>
     <t>10A</t>
@@ -616,9 +604,6 @@
     <t>Sarkar; Raghunath</t>
   </si>
   <si>
-    <t>Vogel B2 (EI Vol. XX, p. 18, plate B2)</t>
-  </si>
-  <si>
     <t>Vogel M3 (EI Vol. XXI, p. 66, plate M-3)</t>
   </si>
   <si>
@@ -1006,9 +991,6 @@
     <t>Vogel 1929-30: 19 (B5). — Raghunath 2001: 83-4 (8).</t>
   </si>
   <si>
-    <t>Raghunath 2001: 82 (7A).</t>
-  </si>
-  <si>
     <t>Store at Nagarjunakonda</t>
   </si>
   <si>
@@ -1055,27 +1037,6 @@
   </si>
   <si>
     <t>No rubbing for our IKS006 in Raghunath. See remark under IKS005.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri (Corps)"/>
-      </rPr>
-      <t xml:space="preserve">estampage Leiden N11. — </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="136"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Raghunath</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1168,9 +1129,6 @@
     </r>
   </si>
   <si>
-    <t>estampage Leiden N8.</t>
-  </si>
-  <si>
     <t>Sankaranarayanan; Raghunath.</t>
   </si>
   <si>
@@ -1200,9 +1158,6 @@
   </si>
   <si>
     <t>estampage Leiden N15 (three separate sheets).</t>
-  </si>
-  <si>
-    <t>south of the Mahācaitya at Nāgārjunakoṇḍa Site-1</t>
   </si>
   <si>
     <t>estampage Leiden N9.</t>
@@ -1334,12 +1289,92 @@
       <t>von Hinüber 2012; 2013.</t>
     </r>
   </si>
+  <si>
+    <t>estampage Leiden N8. — Raghunath.</t>
+  </si>
+  <si>
+    <t>Raghunath 2001: 82 (7A) = 91 (9B).</t>
+  </si>
+  <si>
+    <t>Raghunath 7A lacks rubbing; the same inscription is included again under 9B, there with a rubbing, but one that omits the last line.</t>
+  </si>
+  <si>
+    <t>7A, 9B</t>
+  </si>
+  <si>
+    <t>estampage Leiden N8. — Vogel; Raghunath.</t>
+  </si>
+  <si>
+    <t>Raghunath 2001: 89-90 (9A).</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Corps)"/>
+      </rPr>
+      <t xml:space="preserve">estampage Leiden N11. — </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Raghunath.</t>
+    </r>
+  </si>
+  <si>
+    <t>broken octogonal pillar</t>
+  </si>
+  <si>
+    <t>Dhaṁmasena's donation</t>
+  </si>
+  <si>
+    <t>Naga 11</t>
+  </si>
+  <si>
+    <t>Vogel 1929-30: 18 (B2). — Raghunath 2001: 93-4 (10).</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Corps)"/>
+      </rPr>
+      <t xml:space="preserve">estampage Leiden N8. — </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vogel; Raghunath</t>
+    </r>
+  </si>
+  <si>
+    <t>erection of a pillar for attaining bliss or nirvana</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1422,22 +1457,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1782,10 +1817,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N116"/>
+  <dimension ref="A1:N115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="83" workbookViewId="0">
-      <selection activeCell="M111" sqref="M111"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="83" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1808,26 +1843,26 @@
   <sheetData>
     <row r="1" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="E2" s="2" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="2" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>9</v>
@@ -1876,25 +1911,25 @@
         <v>4</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>13</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="N4" s="4"/>
     </row>
@@ -1909,37 +1944,37 @@
         <v>1</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F5" s="5">
         <v>15</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="H5" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>295</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>294</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>297</v>
-      </c>
       <c r="L5" s="5" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="112" x14ac:dyDescent="0.2">
@@ -1951,34 +1986,34 @@
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="5" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>15</v>
+        <v>363</v>
       </c>
       <c r="F6" s="5">
         <v>4</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="H6" s="5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L6" s="5" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="N6" s="4"/>
     </row>
@@ -1994,31 +2029,31 @@
         <v>1</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F7" s="5">
         <v>13</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="N7" s="4" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="64" x14ac:dyDescent="0.2">
@@ -2030,34 +2065,34 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="5" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F8" s="5">
         <v>12</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="N8" s="4" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -2069,34 +2104,34 @@
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F9" s="5">
         <v>13</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L9" s="5" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="N9" s="4" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -2104,38 +2139,38 @@
         <v>7</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C10" s="5"/>
       <c r="D10" s="5" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F10" s="5">
         <v>5</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="N10" s="4"/>
     </row>
@@ -2148,71 +2183,73 @@
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="5" t="s">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F11" s="5">
         <v>7</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L11" s="5" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="N11" s="4"/>
     </row>
-    <row r="12" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="96" x14ac:dyDescent="0.2">
       <c r="A12" s="5">
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>151</v>
+        <v>359</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="F12" s="4">
-        <v>9</v>
+        <v>293</v>
+      </c>
+      <c r="F12" s="5">
+        <v>10</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>108</v>
+        <v>302</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>340</v>
+        <v>356</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="N12" s="4"/>
+        <v>357</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>358</v>
+      </c>
     </row>
     <row r="13" spans="1:14" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="5">
@@ -2223,34 +2260,34 @@
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="5" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F13" s="5">
         <v>7</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I13" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L13" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="M13" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="K13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>336</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>309</v>
-      </c>
       <c r="N13" s="4" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -2258,35 +2295,35 @@
         <v>11</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>312</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>312</v>
+        <v>306</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>306</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F14" s="5">
         <v>10</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="N14" s="4"/>
     </row>
@@ -2299,134 +2336,138 @@
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="5" t="s">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F15" s="5">
         <v>8</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I15" s="4" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="N15" s="4"/>
     </row>
     <row r="16" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A16" s="4">
+      <c r="A16" s="5">
         <v>13</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>153</v>
+      <c r="B16" s="5" t="s">
+        <v>150</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="D16" s="4" t="s">
+        <v>306</v>
+      </c>
       <c r="E16" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="F16" s="4">
+        <v>293</v>
+      </c>
+      <c r="F16" s="5">
         <v>9</v>
       </c>
       <c r="G16" s="4"/>
-      <c r="H16" s="4" t="s">
-        <v>10</v>
+      <c r="H16" s="5" t="s">
+        <v>287</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L16" s="4" t="s">
-        <v>327</v>
-      </c>
-      <c r="M16" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="L16" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="M16" s="5" t="s">
+        <v>361</v>
       </c>
       <c r="N16" s="4"/>
     </row>
-    <row r="17" spans="1:14" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="4">
+    <row r="17" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="A17" s="5">
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>154</v>
+        <v>306</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="D17" s="4" t="s">
+        <v>306</v>
+      </c>
       <c r="E17" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="F17" s="4">
+        <v>293</v>
+      </c>
+      <c r="F17" s="5">
         <v>10</v>
       </c>
       <c r="G17" s="4"/>
-      <c r="H17" s="4" t="s">
-        <v>10</v>
+      <c r="H17" s="5" t="s">
+        <v>287</v>
       </c>
       <c r="I17" s="4" t="s">
-        <v>108</v>
+        <v>299</v>
       </c>
       <c r="K17" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L17" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="M17" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="N17" s="4"/>
     </row>
     <row r="18" spans="1:14" ht="48" x14ac:dyDescent="0.2">
-      <c r="A18" s="4">
+      <c r="A18" s="5">
         <v>15</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B18" s="5">
         <v>10</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18" s="4">
-        <v>11</v>
+      <c r="D18" s="5" t="s">
+        <v>365</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>298</v>
-      </c>
-      <c r="F18" s="4">
+        <v>293</v>
+      </c>
+      <c r="F18" s="5">
         <v>7</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>251</v>
-      </c>
-      <c r="H18" s="4" t="s">
-        <v>10</v>
+        <v>246</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>287</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="L18" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="M18" s="4" t="s">
-        <v>187</v>
+        <v>17</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="M18" s="5" t="s">
+        <v>366</v>
       </c>
       <c r="N18" s="4"/>
     </row>
@@ -2435,12 +2476,12 @@
         <v>16</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F19" s="4">
         <v>10</v>
@@ -2450,16 +2491,16 @@
         <v>10</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>25</v>
+        <v>368</v>
       </c>
       <c r="L19" s="4" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="M19" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N19" s="4"/>
     </row>
@@ -2468,12 +2509,12 @@
         <v>17</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F20" s="4">
         <v>9</v>
@@ -2483,16 +2524,16 @@
         <v>10</v>
       </c>
       <c r="I20" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K20" s="4" t="s">
         <v>13</v>
       </c>
       <c r="L20" s="4" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="M20" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N20" s="4"/>
     </row>
@@ -2501,12 +2542,12 @@
         <v>18</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F21" s="4">
         <v>10</v>
@@ -2516,16 +2557,16 @@
         <v>10</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K21" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="L21" s="4" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N21" s="4"/>
     </row>
@@ -2534,12 +2575,12 @@
         <v>19</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F22" s="4">
         <v>6</v>
@@ -2549,19 +2590,19 @@
         <v>10</v>
       </c>
       <c r="I22" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K22" s="4" t="s">
         <v>13</v>
       </c>
       <c r="L22" s="4" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="M22" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N22" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="64" x14ac:dyDescent="0.2">
@@ -2576,28 +2617,28 @@
         <v>41</v>
       </c>
       <c r="E23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="K23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="L23" s="4" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="N23" s="4"/>
     </row>
@@ -2623,19 +2664,19 @@
         <v>10</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="L24" s="4" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="N24" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -2643,7 +2684,7 @@
         <v>22</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="4">
@@ -2660,17 +2701,17 @@
         <v>10</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K25" s="4"/>
       <c r="L25" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="M25" s="4" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="N25" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -2678,7 +2719,7 @@
         <v>23</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4">
@@ -2695,17 +2736,17 @@
         <v>10</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K26" s="4"/>
       <c r="L26" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="M26" s="4" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="N26" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -2713,7 +2754,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="C27" s="4"/>
       <c r="D27" s="4">
@@ -2723,24 +2764,24 @@
         <v>12</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I27" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K27" s="4"/>
       <c r="L27" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="M27" s="4" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="N27" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -2748,7 +2789,7 @@
         <v>25</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28" s="4">
@@ -2765,19 +2806,19 @@
         <v>10</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="N28" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -2785,7 +2826,7 @@
         <v>26</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C29" s="4"/>
       <c r="D29" s="4">
@@ -2802,19 +2843,19 @@
         <v>10</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K29" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="N29" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -2822,11 +2863,11 @@
         <v>27</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="C30" s="4"/>
       <c r="D30" s="4" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4">
@@ -2837,18 +2878,18 @@
         <v>10</v>
       </c>
       <c r="I30" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="K30" s="4"/>
       <c r="L30" s="4"/>
       <c r="M30" s="4" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="N30" s="4" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -2863,28 +2904,28 @@
         <v>18</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F31" s="4">
         <v>2</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="H31" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I31" s="4" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="K31" s="4" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="N31" s="4"/>
     </row>
@@ -2900,7 +2941,7 @@
         <v>1</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F32" s="4">
         <v>10</v>
@@ -2910,19 +2951,19 @@
         <v>10</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="K32" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="N32" s="4"/>
     </row>
@@ -2948,16 +2989,16 @@
         <v>10</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="K33" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="N33" s="4"/>
     </row>
@@ -2966,14 +3007,14 @@
         <v>31</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="C34" s="4"/>
       <c r="D34" s="4">
         <v>3</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F34" s="4">
         <v>6</v>
@@ -2983,17 +3024,17 @@
         <v>10</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K34" s="4" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="L34" s="4"/>
       <c r="M34" s="4" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="N34" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="80" x14ac:dyDescent="0.2">
@@ -3018,15 +3059,15 @@
         <v>10</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K35" s="4"/>
       <c r="L35" s="4"/>
       <c r="M35" s="4" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="N35" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="80" x14ac:dyDescent="0.2">
@@ -3034,7 +3075,7 @@
         <v>33</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4">
@@ -3051,17 +3092,17 @@
         <v>10</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="L36" s="4"/>
       <c r="M36" s="4" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="N36" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3074,7 +3115,7 @@
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F37" s="4">
         <v>10</v>
@@ -3084,17 +3125,17 @@
         <v>10</v>
       </c>
       <c r="I37" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K37" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="L37" s="4"/>
       <c r="M37" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="N37" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -3102,7 +3143,7 @@
         <v>35</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C38" s="4"/>
       <c r="D38" s="4">
@@ -3119,19 +3160,19 @@
         <v>10</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="L38" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="M38" s="4" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="N38" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -3146,7 +3187,7 @@
         <v>66</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F39" s="4">
         <v>2</v>
@@ -3156,17 +3197,17 @@
         <v>10</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K39" s="4"/>
       <c r="L39" s="4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="N39" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -3191,17 +3232,17 @@
         <v>10</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K40" s="4"/>
       <c r="L40" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="N40" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -3226,17 +3267,17 @@
         <v>10</v>
       </c>
       <c r="I41" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K41" s="4"/>
       <c r="L41" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="N41" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3261,16 +3302,16 @@
         <v>10</v>
       </c>
       <c r="I42" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K42" s="4" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="N42" s="4"/>
     </row>
@@ -3296,16 +3337,16 @@
         <v>10</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="N43" s="4"/>
     </row>
@@ -3314,11 +3355,11 @@
         <v>41</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C44" s="4"/>
       <c r="D44" s="4" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>12</v>
@@ -3328,13 +3369,13 @@
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="4" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I44" s="4"/>
       <c r="K44" s="4"/>
       <c r="L44" s="4"/>
       <c r="M44" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N44" s="4"/>
     </row>
@@ -3360,17 +3401,17 @@
         <v>10</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K45" s="4"/>
       <c r="L45" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="N45" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -3395,14 +3436,14 @@
         <v>10</v>
       </c>
       <c r="I46" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K46" s="4"/>
       <c r="L46" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="N46" s="4"/>
     </row>
@@ -3418,28 +3459,28 @@
         <v>44</v>
       </c>
       <c r="E47" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="F47" s="4">
+        <v>10</v>
+      </c>
+      <c r="G47" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I47" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="F47" s="4">
-        <v>10</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="I47" s="4" t="s">
-        <v>306</v>
-      </c>
       <c r="K47" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L47" s="4" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="M47" s="4" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="N47" s="4"/>
     </row>
@@ -3455,7 +3496,7 @@
         <v>43</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="F48" s="4">
         <v>14</v>
@@ -3465,16 +3506,16 @@
         <v>10</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K48" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="L48" s="4" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="M48" s="4" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="N48" s="4"/>
     </row>
@@ -3490,7 +3531,7 @@
         <v>42</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="F49" s="4">
         <v>8</v>
@@ -3500,16 +3541,16 @@
         <v>10</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="K49" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="L49" s="4" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="M49" s="4" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="N49" s="4"/>
     </row>
@@ -3525,31 +3566,31 @@
         <v>53</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F50" s="4">
         <v>17</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="H50" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="K50" s="4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="N50" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -3564,31 +3605,31 @@
         <v>54</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F51" s="4">
         <v>17</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="H51" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="K51" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="N51" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -3600,34 +3641,34 @@
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="E52" s="4" t="s">
         <v>293</v>
-      </c>
-      <c r="E52" s="4" t="s">
-        <v>298</v>
       </c>
       <c r="F52" s="4">
         <v>12</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="H52" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="N52" s="4"/>
     </row>
@@ -3641,29 +3682,29 @@
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F53" s="4">
         <v>6</v>
       </c>
       <c r="G53" s="4"/>
       <c r="H53" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I53" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K53" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="L53" s="4" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="M53" s="4" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="N53" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -3678,31 +3719,31 @@
         <v>45</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F54" s="4">
         <v>14</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="H54" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="K54" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L54" s="4" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="M54" s="4" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="N54" s="4" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="64" x14ac:dyDescent="0.2">
@@ -3721,22 +3762,22 @@
         <v>7</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="H55" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="K55" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="L55" s="4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M55" s="4" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="N55" s="4"/>
     </row>
@@ -3750,26 +3791,26 @@
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="F56" s="4">
         <v>12</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="H56" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K56" s="4"/>
       <c r="L56" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="M56" s="4" t="s">
         <v>228</v>
-      </c>
-      <c r="M56" s="4" t="s">
-        <v>233</v>
       </c>
       <c r="N56" s="4"/>
     </row>
@@ -3785,28 +3826,28 @@
         <v>55</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F57" s="4">
         <v>1</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="H57" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K57" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="L57" s="4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M57" s="4" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="N57" s="4"/>
     </row>
@@ -3815,12 +3856,12 @@
         <v>55</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F58" s="4">
         <v>26</v>
@@ -3830,14 +3871,14 @@
         <v>10</v>
       </c>
       <c r="I58" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="K58" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L58" s="4"/>
       <c r="M58" s="5" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="N58" s="4"/>
     </row>
@@ -3851,7 +3892,7 @@
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F59" s="4">
         <v>7</v>
@@ -3861,14 +3902,14 @@
         <v>10</v>
       </c>
       <c r="I59" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K59" s="4"/>
       <c r="L59" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M59" s="4" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="N59" s="4"/>
     </row>
@@ -3882,7 +3923,7 @@
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F60" s="4">
         <v>4</v>
@@ -3892,16 +3933,16 @@
         <v>10</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="K60" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L60" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M60" s="4" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="N60" s="4"/>
     </row>
@@ -3917,26 +3958,26 @@
         <v>10</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F61" s="4">
         <v>6</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="H61" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I61" s="4" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="K61" s="4"/>
       <c r="L61" s="4" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="M61" s="4" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="N61" s="4"/>
     </row>
@@ -3952,7 +3993,7 @@
         <v>62</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F62" s="4">
         <v>1</v>
@@ -3962,16 +4003,16 @@
         <v>10</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="K62" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="L62" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="M62" s="4" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="N62" s="4"/>
     </row>
@@ -3987,7 +4028,7 @@
         <v>51</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F63" s="4">
         <v>8</v>
@@ -3997,16 +4038,16 @@
         <v>10</v>
       </c>
       <c r="I63" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K63" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="L63" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M63" s="4" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="N63" s="4"/>
     </row>
@@ -4022,7 +4063,7 @@
         <v>50</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F64" s="4">
         <v>3</v>
@@ -4032,16 +4073,16 @@
         <v>10</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K64" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M64" s="4" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="N64" s="4"/>
     </row>
@@ -4055,7 +4096,7 @@
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
       <c r="E65" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F65" s="4">
         <v>4</v>
@@ -4065,14 +4106,14 @@
         <v>10</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="K65" s="4"/>
       <c r="L65" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M65" s="4" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="N65" s="4"/>
     </row>
@@ -4086,7 +4127,7 @@
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
       <c r="E66" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F66" s="4">
         <v>2</v>
@@ -4096,16 +4137,16 @@
         <v>10</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K66" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L66" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M66" s="4" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="N66" s="4"/>
     </row>
@@ -4121,7 +4162,7 @@
         <v>59</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F67" s="4">
         <v>5</v>
@@ -4131,16 +4172,16 @@
         <v>10</v>
       </c>
       <c r="I67" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K67" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="L67" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M67" s="4" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="N67" s="4"/>
     </row>
@@ -4154,7 +4195,7 @@
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
       <c r="E68" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F68" s="4">
         <v>6</v>
@@ -4162,15 +4203,15 @@
       <c r="G68" s="4"/>
       <c r="H68" s="4"/>
       <c r="I68" s="4" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="K68" s="4"/>
       <c r="L68" s="4"/>
       <c r="M68" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="N68" s="4"/>
     </row>
@@ -4184,7 +4225,7 @@
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
       <c r="E69" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F69" s="4">
         <v>2</v>
@@ -4192,12 +4233,12 @@
       <c r="G69" s="4"/>
       <c r="H69" s="4"/>
       <c r="I69" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K69" s="4"/>
       <c r="L69" s="4"/>
       <c r="M69" s="4" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="N69" s="4"/>
     </row>
@@ -4211,7 +4252,7 @@
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
       <c r="E70" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F70" s="4">
         <v>5</v>
@@ -4219,12 +4260,12 @@
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="I70" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="K70" s="4"/>
       <c r="L70" s="4"/>
       <c r="M70" s="4" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="N70" s="4"/>
     </row>
@@ -4238,28 +4279,28 @@
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
       <c r="E71" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F71" s="4">
         <v>5</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="H71" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I71" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K71" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L71" s="4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M71" s="4" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="N71" s="4"/>
     </row>
@@ -4273,7 +4314,7 @@
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
       <c r="E72" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F72" s="4">
         <v>6</v>
@@ -4281,16 +4322,16 @@
       <c r="G72" s="4"/>
       <c r="H72" s="4"/>
       <c r="I72" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K72" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L72" s="4" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="M72" s="4" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="N72" s="4"/>
     </row>
@@ -4304,7 +4345,7 @@
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
       <c r="E73" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F73" s="4">
         <v>3</v>
@@ -4314,16 +4355,16 @@
         <v>10</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="K73" s="4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L73" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M73" s="4" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="N73" s="4"/>
     </row>
@@ -4337,7 +4378,7 @@
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
       <c r="E74" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F74" s="4">
         <v>3</v>
@@ -4347,16 +4388,16 @@
         <v>10</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K74" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L74" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M74" s="4" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="N74" s="4"/>
     </row>
@@ -4370,7 +4411,7 @@
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
       <c r="E75" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F75" s="4">
         <v>3</v>
@@ -4380,16 +4421,16 @@
         <v>10</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K75" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L75" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M75" s="4" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="N75" s="4"/>
     </row>
@@ -4403,7 +4444,7 @@
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
       <c r="E76" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F76" s="4">
         <v>4</v>
@@ -4413,16 +4454,16 @@
         <v>10</v>
       </c>
       <c r="I76" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="K76" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M76" s="4" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="N76" s="4"/>
     </row>
@@ -4438,7 +4479,7 @@
         <v>57</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F77" s="4">
         <v>2</v>
@@ -4448,16 +4489,16 @@
         <v>10</v>
       </c>
       <c r="I77" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="K77" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L77" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M77" s="4" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="N77" s="4"/>
     </row>
@@ -4471,7 +4512,7 @@
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
       <c r="E78" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F78" s="4">
         <v>5</v>
@@ -4481,16 +4522,16 @@
         <v>10</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="K78" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="L78" s="4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M78" s="4" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="N78" s="4"/>
     </row>
@@ -4504,7 +4545,7 @@
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
       <c r="E79" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F79" s="4">
         <v>3</v>
@@ -4514,16 +4555,16 @@
         <v>10</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K79" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="L79" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M79" s="4" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="N79" s="4"/>
     </row>
@@ -4539,29 +4580,29 @@
         <v>56</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F80" s="4">
         <v>5</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="H80" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K80" s="4"/>
       <c r="L80" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="M80" s="4" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="N80" s="4" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
     </row>
     <row r="81" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -4569,12 +4610,12 @@
         <v>78</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
       <c r="E81" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F81" s="4">
         <v>3</v>
@@ -4582,14 +4623,14 @@
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
       <c r="I81" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K81" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L81" s="4"/>
       <c r="M81" s="4" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="N81" s="4"/>
     </row>
@@ -4605,7 +4646,7 @@
         <v>48</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F82" s="4">
         <v>3</v>
@@ -4613,19 +4654,19 @@
       <c r="G82" s="4"/>
       <c r="H82" s="4"/>
       <c r="I82" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K82" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L82" s="4" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="M82" s="4" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="N82" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="83" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -4640,26 +4681,26 @@
         <v>46</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="F83" s="4">
         <v>2</v>
       </c>
       <c r="G83" s="4" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="H83" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="K83" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L83" s="4"/>
       <c r="M83" s="4" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="N83" s="4"/>
     </row>
@@ -4675,26 +4716,26 @@
         <v>47</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F84" s="4">
         <v>1</v>
       </c>
       <c r="G84" s="4" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="H84" s="4" t="s">
         <v>10</v>
       </c>
       <c r="I84" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K84" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L84" s="4"/>
       <c r="M84" s="4" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="N84" s="4"/>
     </row>
@@ -4720,19 +4761,19 @@
         <v>10</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="K85" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L85" s="4" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="M85" s="4" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="N85" s="4"/>
     </row>
@@ -4758,16 +4799,16 @@
         <v>10</v>
       </c>
       <c r="I86" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K86" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="L86" s="4" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="M86" s="4" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="N86" s="4"/>
     </row>
@@ -4783,7 +4824,7 @@
         <v>70</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F87" s="4">
         <v>9</v>
@@ -4791,19 +4832,19 @@
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K87" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="L87" s="4" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="M87" s="4" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="N87" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="88" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -4816,7 +4857,7 @@
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
       <c r="E88" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F88" s="4">
         <v>1</v>
@@ -4824,12 +4865,12 @@
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
       <c r="I88" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K88" s="4"/>
       <c r="L88" s="4"/>
       <c r="M88" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="N88" s="4"/>
     </row>
@@ -4843,7 +4884,7 @@
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
       <c r="E89" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F89" s="4">
         <v>2</v>
@@ -4851,12 +4892,12 @@
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
       <c r="I89" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K89" s="4"/>
       <c r="L89" s="4"/>
       <c r="M89" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="N89" s="4"/>
     </row>
@@ -4870,7 +4911,7 @@
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
       <c r="E90" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F90" s="4">
         <v>1</v>
@@ -4878,15 +4919,15 @@
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K90" s="4"/>
       <c r="L90" s="4"/>
       <c r="M90" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="N90" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="91" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -4899,7 +4940,7 @@
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
       <c r="E91" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F91" s="4">
         <v>2</v>
@@ -4907,15 +4948,15 @@
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
       <c r="I91" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K91" s="4"/>
       <c r="L91" s="4"/>
       <c r="M91" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="N91" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.2">
@@ -4928,7 +4969,7 @@
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
       <c r="E92" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F92" s="4">
         <v>2</v>
@@ -4936,15 +4977,15 @@
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
       <c r="I92" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="K92" s="4"/>
       <c r="L92" s="4"/>
       <c r="M92" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="N92" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.2">
@@ -4963,15 +5004,15 @@
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
       <c r="I93" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="K93" s="4"/>
       <c r="L93" s="4"/>
       <c r="M93" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="N93" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="94" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -4990,15 +5031,15 @@
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
       <c r="I94" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K94" s="4"/>
       <c r="L94" s="4"/>
       <c r="M94" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="N94" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.2">
@@ -5011,7 +5052,7 @@
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
       <c r="E95" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F95" s="4">
         <v>3</v>
@@ -5019,15 +5060,15 @@
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
       <c r="I95" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="K95" s="4"/>
       <c r="L95" s="4"/>
       <c r="M95" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="N95" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="96" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5040,7 +5081,7 @@
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
       <c r="E96" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F96" s="4">
         <v>4</v>
@@ -5048,7 +5089,7 @@
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
       <c r="I96" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="K96" s="4"/>
       <c r="L96" s="4"/>
@@ -5065,7 +5106,7 @@
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
       <c r="E97" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F97" s="4">
         <v>1</v>
@@ -5073,12 +5114,12 @@
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="K97" s="4"/>
       <c r="L97" s="4"/>
       <c r="M97" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="N97" s="4"/>
     </row>
@@ -5098,15 +5139,15 @@
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
       <c r="I98" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="K98" s="4"/>
       <c r="L98" s="4"/>
       <c r="M98" s="4" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="N98" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="99" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -5121,7 +5162,7 @@
         <v>64</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F99" s="4">
         <v>1</v>
@@ -5134,11 +5175,11 @@
         <v>11</v>
       </c>
       <c r="K99" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L99" s="4"/>
       <c r="M99" s="4" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="N99" s="4"/>
     </row>
@@ -5154,7 +5195,7 @@
         <v>1</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F100" s="4">
         <v>3</v>
@@ -5164,19 +5205,19 @@
         <v>10</v>
       </c>
       <c r="I100" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="J100" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="K100" s="4" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="L100" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="M100" s="4" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="N100" s="4"/>
     </row>
@@ -5192,7 +5233,7 @@
         <v>2</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F101" s="4">
         <v>3</v>
@@ -5202,19 +5243,19 @@
         <v>10</v>
       </c>
       <c r="I101" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J101" s="7" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="K101" s="4" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="L101" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="M101" s="4" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="N101" s="4"/>
     </row>
@@ -5230,7 +5271,7 @@
         <v>3</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F102" s="4">
         <v>1</v>
@@ -5240,17 +5281,17 @@
         <v>10</v>
       </c>
       <c r="I102" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J102" s="7" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="K102" s="4"/>
       <c r="L102" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="M102" s="4" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="N102" s="4"/>
     </row>
@@ -5274,20 +5315,20 @@
         <v>10</v>
       </c>
       <c r="I103" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J103" s="7" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="K103" s="4"/>
       <c r="L103" s="4" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="M103" s="4" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="N103" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
@@ -5300,7 +5341,7 @@
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
       <c r="E104" s="4" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F104" s="4">
         <v>1</v>
@@ -5308,14 +5349,14 @@
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
       <c r="I104" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K104" s="4"/>
       <c r="L104" s="4" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="M104" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N104" s="4"/>
     </row>
@@ -5329,7 +5370,7 @@
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
       <c r="E105" s="4" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F105" s="4">
         <v>6</v>
@@ -5337,14 +5378,14 @@
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
       <c r="I105" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="K105" s="4"/>
       <c r="L105" s="4" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="M105" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="N105" s="4"/>
     </row>
@@ -5358,7 +5399,7 @@
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
       <c r="E106" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F106" s="4">
         <v>1</v>
@@ -5366,7 +5407,7 @@
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
       <c r="I106" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K106" s="4"/>
       <c r="L106" s="4"/>
@@ -5378,31 +5419,31 @@
         <v>104</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F107" s="1">
         <v>11</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>346</v>
+        <v>338</v>
       </c>
       <c r="J107" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="L107" s="1" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="M107" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="108" spans="1:14" ht="48" x14ac:dyDescent="0.2">
@@ -5410,118 +5451,112 @@
         <v>105</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="F108" s="1">
         <v>10</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I108" s="1" t="s">
-        <v>348</v>
+        <v>300</v>
       </c>
       <c r="J108" s="1" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="L108" s="1" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="M108" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="109" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="109" spans="1:14" ht="80" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>106</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>298</v>
+        <v>12</v>
       </c>
       <c r="F109" s="1">
         <v>10</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>292</v>
+        <v>348</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="J109" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="L109" s="1" t="s">
-        <v>347</v>
+        <v>349</v>
+      </c>
+      <c r="J109" s="4" t="s">
+        <v>350</v>
       </c>
       <c r="M109" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="110" spans="1:14" ht="80" x14ac:dyDescent="0.2">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="110" spans="1:14" ht="64" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>107</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="E110" s="1" t="s">
         <v>12</v>
       </c>
       <c r="F110" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>357</v>
+        <v>287</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="J110" s="4" t="s">
-        <v>359</v>
-      </c>
-      <c r="M110" s="1" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="111" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+        <v>349</v>
+      </c>
+      <c r="K110" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="M110" s="4" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" ht="32" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>108</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="E111" s="1" t="s">
-        <v>12</v>
+        <v>306</v>
       </c>
       <c r="F111" s="1">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="H111" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I111" s="1" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="M111" s="4" t="s">
-        <v>364</v>
+        <v>354</v>
       </c>
     </row>
     <row r="112" spans="1:14" ht="32" x14ac:dyDescent="0.2">
@@ -5529,22 +5564,22 @@
         <v>109</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="F112" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H112" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="M112" s="4" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
     </row>
     <row r="113" spans="1:13" ht="32" x14ac:dyDescent="0.2">
@@ -5552,59 +5587,36 @@
         <v>110</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="F113" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H113" s="1" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
       <c r="M113" s="4" t="s">
-        <v>363</v>
+        <v>354</v>
       </c>
     </row>
     <row r="114" spans="1:13" ht="32" x14ac:dyDescent="0.2">
-      <c r="A114" s="1">
-        <v>111</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="D114" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="F114" s="1">
-        <v>3</v>
-      </c>
-      <c r="H114" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="I114" s="1" t="s">
-        <v>358</v>
-      </c>
-      <c r="M114" s="4" t="s">
-        <v>363</v>
-      </c>
-    </row>
-    <row r="115" spans="1:13" ht="32" x14ac:dyDescent="0.2">
+      <c r="A114" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A116" s="1" t="s">
-        <v>362</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>

</xml_diff>